<commit_message>
Tech units of installation
New variables:
-exogenous = cap_units
-endogenous_integer = new_units
</commit_message>
<xml_diff>
--- a/thesis/main_new_formulation_int/input_data/input_data.xlsx
+++ b/thesis/main_new_formulation_int/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_tesi/thesis/main_new_formulation_int/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25ABA80-3050-434E-9455-69DBD6B31682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B6B144-6D69-6645-9274-BAB6B3F180AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="u" sheetId="1" r:id="rId1"/>
@@ -20,29 +20,30 @@
     <sheet name="cost_op" sheetId="5" r:id="rId5"/>
     <sheet name="cost_inv" sheetId="6" r:id="rId6"/>
     <sheet name="cap_i" sheetId="7" r:id="rId7"/>
-    <sheet name="Act_constr" sheetId="8" r:id="rId8"/>
-    <sheet name="days_per_type" sheetId="9" r:id="rId9"/>
-    <sheet name="sf" sheetId="10" r:id="rId10"/>
-    <sheet name="TI_param" sheetId="11" r:id="rId11"/>
-    <sheet name="TI_cost" sheetId="12" r:id="rId12"/>
-    <sheet name="storage_min" sheetId="13" r:id="rId13"/>
-    <sheet name="storage_max" sheetId="14" r:id="rId14"/>
-    <sheet name="storage_start" sheetId="15" r:id="rId15"/>
-    <sheet name="storage_max_disch" sheetId="16" r:id="rId16"/>
-    <sheet name="storage_min_charge" sheetId="17" r:id="rId17"/>
-    <sheet name="BEV_level_min" sheetId="19" r:id="rId18"/>
-    <sheet name="BEV_level_max" sheetId="20" r:id="rId19"/>
-    <sheet name="BEV_level_start" sheetId="21" r:id="rId20"/>
-    <sheet name="BEV_vector" sheetId="22" r:id="rId21"/>
-    <sheet name="loss_factors" sheetId="23" r:id="rId22"/>
-    <sheet name="n_hours" sheetId="24" r:id="rId23"/>
+    <sheet name="cap_unit" sheetId="25" r:id="rId8"/>
+    <sheet name="Act_constr" sheetId="8" r:id="rId9"/>
+    <sheet name="days_per_type" sheetId="9" r:id="rId10"/>
+    <sheet name="sf" sheetId="10" r:id="rId11"/>
+    <sheet name="TI_param" sheetId="11" r:id="rId12"/>
+    <sheet name="TI_cost" sheetId="12" r:id="rId13"/>
+    <sheet name="storage_min" sheetId="13" r:id="rId14"/>
+    <sheet name="storage_max" sheetId="14" r:id="rId15"/>
+    <sheet name="storage_start" sheetId="15" r:id="rId16"/>
+    <sheet name="storage_max_disch" sheetId="16" r:id="rId17"/>
+    <sheet name="storage_min_charge" sheetId="17" r:id="rId18"/>
+    <sheet name="BEV_level_min" sheetId="19" r:id="rId19"/>
+    <sheet name="BEV_level_max" sheetId="20" r:id="rId20"/>
+    <sheet name="BEV_level_start" sheetId="21" r:id="rId21"/>
+    <sheet name="BEV_vector" sheetId="22" r:id="rId22"/>
+    <sheet name="loss_factors" sheetId="23" r:id="rId23"/>
+    <sheet name="n_hours" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6349" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6389" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -4955,6 +4956,75 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E162"/>
   <sheetViews>
@@ -7283,7 +7353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -7464,7 +7534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -7499,7 +7569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -7732,7 +7802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -7965,7 +8035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -8198,7 +8268,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E127"/>
   <sheetViews>
@@ -10036,7 +10106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E127"/>
   <sheetViews>
@@ -11874,7 +11944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -12064,236 +12134,6 @@
       </c>
       <c r="D16">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16">
-        <v>0.95</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -16668,6 +16508,236 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -16897,11 +16967,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:E415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+    <sheetView topLeftCell="A310" workbookViewId="0">
       <selection activeCell="O339" sqref="O339"/>
     </sheetView>
   </sheetViews>
@@ -23971,7 +24041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -24252,7 +24322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -28666,6 +28736,287 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282BC33A-597F-F14E-8267-14D242F3BCF5}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E415"/>
   <sheetViews>
@@ -35731,73 +36082,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>